<commit_message>
Edit task sheet Finish report 200 page Add Appendix report full
</commit_message>
<xml_diff>
--- a/doc/Tasksheet.xlsx
+++ b/doc/Tasksheet.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="137">
   <si>
     <t>No.</t>
   </si>
@@ -373,24 +373,6 @@
     <t>Interaction Diagram</t>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;Guest&gt; Squence Diagram</t>
-  </si>
-  <si>
-    <t>&lt;Customer&gt; Squence Diagram</t>
-  </si>
-  <si>
-    <t>&lt;Staff&gt; Squence Diagram</t>
-  </si>
-  <si>
-    <t>&lt;Admin&gt; Squence Diagram</t>
-  </si>
-  <si>
-    <t>&lt;Manager&gt; Squence Diagram</t>
-  </si>
-  <si>
-    <t>&lt;System&gt; Squence Diagram</t>
-  </si>
-  <si>
     <t>User Interface Design</t>
   </si>
   <si>
@@ -505,9 +487,6 @@
     <t>Overview</t>
   </si>
   <si>
-    <t>Setup Environtment</t>
-  </si>
-  <si>
     <t>Coding admin functions</t>
   </si>
   <si>
@@ -547,9 +526,6 @@
     <t>Manage amenity</t>
   </si>
   <si>
-    <t>Statistics and Calendar</t>
-  </si>
-  <si>
     <t>Customer functions</t>
   </si>
   <si>
@@ -604,10 +580,40 @@
     <t>Suggest office</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Manage amenity group</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Login / Log out</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;Guest&gt; Sequence  Diagram</t>
+  </si>
+  <si>
+    <t>&lt;Customer&gt; Sequence  Diagram</t>
+  </si>
+  <si>
+    <t>&lt;Staff&gt; Sequence  Diagram</t>
+  </si>
+  <si>
+    <t>&lt;Admin&gt; Sequence  Diagram</t>
+  </si>
+  <si>
+    <t>&lt;Manager&gt; Sequence  Diagram</t>
+  </si>
+  <si>
+    <t>&lt;System&gt; Sequence  Diagram</t>
+  </si>
+  <si>
+    <t>Setup Environment</t>
   </si>
 </sst>
 </file>
@@ -844,9 +850,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -857,6 +860,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1167,11 +1173,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I137"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E124" sqref="E124"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1195,16 +1201,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>23</v>
@@ -1214,10 +1220,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="27">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1233,8 +1239,8 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="13" t="s">
         <v>32</v>
       </c>
@@ -1248,8 +1254,8 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
@@ -1263,8 +1269,8 @@
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1278,8 +1284,8 @@
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="15.75">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
@@ -1291,8 +1297,8 @@
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" ht="15.75">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="6" t="s">
         <v>35</v>
       </c>
@@ -1306,8 +1312,8 @@
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" ht="15.75">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
@@ -1327,8 +1333,8 @@
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" ht="15.75">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="4" t="s">
         <v>37</v>
       </c>
@@ -1342,8 +1348,8 @@
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="15.75">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
       <c r="C13" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
@@ -1409,7 +1415,7 @@
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
       <c r="C14" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -1424,7 +1430,7 @@
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
       <c r="C15" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
@@ -1452,7 +1458,7 @@
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -1469,7 +1475,7 @@
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -1486,7 +1492,7 @@
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
@@ -1707,10 +1713,10 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="15.75">
-      <c r="A33" s="27">
+      <c r="A33" s="26">
         <v>4</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -1728,8 +1734,8 @@
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" ht="15.75">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="9" t="s">
         <v>47</v>
       </c>
@@ -1743,8 +1749,8 @@
       <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" ht="15.75">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="9" t="s">
         <v>18</v>
       </c>
@@ -1758,8 +1764,8 @@
       <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" ht="15.75">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="21" t="s">
         <v>48</v>
       </c>
@@ -1771,8 +1777,8 @@
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="1:9" ht="15.75">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="7" t="s">
         <v>49</v>
       </c>
@@ -1784,10 +1790,10 @@
       <c r="I37" s="12"/>
     </row>
     <row r="38" spans="1:9" ht="15.75">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>8</v>
@@ -1801,8 +1807,8 @@
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" ht="15.75">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="8" t="s">
         <v>50</v>
       </c>
@@ -1818,8 +1824,8 @@
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" ht="15.75">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8" t="s">
         <v>51</v>
       </c>
@@ -1833,8 +1839,8 @@
       <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" ht="15.75">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="8" t="s">
         <v>52</v>
       </c>
@@ -1848,8 +1854,8 @@
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="1:9" ht="15.75">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="8" t="s">
         <v>53</v>
       </c>
@@ -1863,8 +1869,8 @@
       <c r="I42" s="12"/>
     </row>
     <row r="43" spans="1:9" ht="15.75">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="8" t="s">
         <v>54</v>
       </c>
@@ -1878,8 +1884,8 @@
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" ht="15.75">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="7" t="s">
         <v>55</v>
       </c>
@@ -1891,10 +1897,10 @@
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" ht="15.75">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="8" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1906,10 +1912,10 @@
       <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" ht="15.75">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="8" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
@@ -1923,10 +1929,10 @@
       <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9" ht="15.75">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>8</v>
@@ -1938,10 +1944,10 @@
       <c r="I47" s="12"/>
     </row>
     <row r="48" spans="1:9" ht="15.75">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="8" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1953,10 +1959,10 @@
       <c r="I48" s="12"/>
     </row>
     <row r="49" spans="1:9" ht="15.75">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
       <c r="C49" s="8" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>8</v>
@@ -1972,10 +1978,10 @@
       <c r="I49" s="12"/>
     </row>
     <row r="50" spans="1:9" ht="15.75">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="8" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>8</v>
@@ -1989,10 +1995,10 @@
       <c r="I50" s="12"/>
     </row>
     <row r="51" spans="1:9" ht="15.75">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2002,10 +2008,10 @@
       <c r="I51" s="12"/>
     </row>
     <row r="52" spans="1:9" ht="15.75">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>8</v>
@@ -2021,10 +2027,10 @@
       <c r="I52" s="12"/>
     </row>
     <row r="53" spans="1:9" ht="15.75">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>8</v>
@@ -2040,10 +2046,10 @@
       <c r="I53" s="12"/>
     </row>
     <row r="54" spans="1:9" ht="15.75">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>8</v>
@@ -2061,10 +2067,10 @@
       <c r="I54" s="12"/>
     </row>
     <row r="55" spans="1:9" ht="15.75">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>8</v>
@@ -2076,10 +2082,10 @@
       <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:9" ht="15.75">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="21" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2089,10 +2095,10 @@
       <c r="I56" s="12"/>
     </row>
     <row r="57" spans="1:9" ht="15.75">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2104,10 +2110,10 @@
       <c r="I57" s="12"/>
     </row>
     <row r="58" spans="1:9" ht="15.75">
-      <c r="A58" s="28"/>
-      <c r="B58" s="28"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
       <c r="C58" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
@@ -2119,8 +2125,8 @@
       <c r="I58" s="12"/>
     </row>
     <row r="59" spans="1:9" ht="15.75">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
       <c r="C59" s="21" t="s">
         <v>21</v>
       </c>
@@ -2132,10 +2138,10 @@
       <c r="I59" s="12"/>
     </row>
     <row r="60" spans="1:9" ht="15.75">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>8</v>
@@ -2147,10 +2153,10 @@
       <c r="I60" s="12"/>
     </row>
     <row r="61" spans="1:9" ht="15.75">
-      <c r="A61" s="29"/>
-      <c r="B61" s="29"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>8</v>
@@ -2162,14 +2168,14 @@
       <c r="I61" s="12"/>
     </row>
     <row r="62" spans="1:9" ht="15.75">
-      <c r="A62" s="30">
+      <c r="A62" s="29">
         <v>5</v>
       </c>
-      <c r="B62" s="27" t="s">
-        <v>72</v>
+      <c r="B62" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>8</v>
@@ -2181,10 +2187,10 @@
       <c r="I62" s="12"/>
     </row>
     <row r="63" spans="1:9" ht="15.75">
-      <c r="A63" s="26"/>
-      <c r="B63" s="28"/>
+      <c r="A63" s="30"/>
+      <c r="B63" s="27"/>
       <c r="C63" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -2194,10 +2200,10 @@
       <c r="I63" s="12"/>
     </row>
     <row r="64" spans="1:9" ht="15.75">
-      <c r="A64" s="26"/>
-      <c r="B64" s="28"/>
+      <c r="A64" s="30"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2205,14 +2211,18 @@
       <c r="G64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
+      <c r="H64" s="12">
+        <v>1</v>
+      </c>
+      <c r="I64" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:9" ht="15.75">
-      <c r="A65" s="26"/>
-      <c r="B65" s="28"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -2220,14 +2230,18 @@
       <c r="G65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
+      <c r="H65" s="12">
+        <v>3</v>
+      </c>
+      <c r="I65" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:9" ht="15.75">
-      <c r="A66" s="26"/>
-      <c r="B66" s="28"/>
+      <c r="A66" s="30"/>
+      <c r="B66" s="27"/>
       <c r="C66" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2237,10 +2251,10 @@
       <c r="I66" s="12"/>
     </row>
     <row r="67" spans="1:9" ht="15.75">
-      <c r="A67" s="26"/>
-      <c r="B67" s="28"/>
+      <c r="A67" s="30"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
@@ -2248,14 +2262,18 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
+      <c r="H67" s="12">
+        <v>2</v>
+      </c>
+      <c r="I67" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="68" spans="1:9" ht="15.75">
-      <c r="A68" s="26"/>
-      <c r="B68" s="28"/>
+      <c r="A68" s="30"/>
+      <c r="B68" s="27"/>
       <c r="C68" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
@@ -2263,14 +2281,18 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
+      <c r="H68" s="12">
+        <v>2</v>
+      </c>
+      <c r="I68" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="69" spans="1:9" ht="15.75">
-      <c r="A69" s="26"/>
-      <c r="B69" s="28"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="27"/>
       <c r="C69" s="10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -2278,14 +2300,18 @@
         <v>8</v>
       </c>
       <c r="G69" s="2"/>
-      <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
+      <c r="H69" s="12">
+        <v>2</v>
+      </c>
+      <c r="I69" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="70" spans="1:9" ht="15.75">
-      <c r="A70" s="26"/>
-      <c r="B70" s="28"/>
+      <c r="A70" s="30"/>
+      <c r="B70" s="27"/>
       <c r="C70" s="10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>8</v>
@@ -2293,14 +2319,18 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
+      <c r="H70" s="12">
+        <v>2</v>
+      </c>
+      <c r="I70" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="71" spans="1:9" ht="15.75">
-      <c r="A71" s="26"/>
-      <c r="B71" s="28"/>
+      <c r="A71" s="30"/>
+      <c r="B71" s="27"/>
       <c r="C71" s="10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -2308,14 +2338,18 @@
         <v>8</v>
       </c>
       <c r="G71" s="2"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
+      <c r="H71" s="12">
+        <v>2</v>
+      </c>
+      <c r="I71" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" spans="1:9" ht="15.75">
-      <c r="A72" s="26"/>
-      <c r="B72" s="28"/>
+      <c r="A72" s="30"/>
+      <c r="B72" s="27"/>
       <c r="C72" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -2323,14 +2357,18 @@
       <c r="G72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
+      <c r="H72" s="12">
+        <v>2</v>
+      </c>
+      <c r="I72" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="73" spans="1:9" ht="15.75">
-      <c r="A73" s="26"/>
-      <c r="B73" s="28"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="27"/>
       <c r="C73" s="10" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -2338,76 +2376,96 @@
       <c r="G73" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
+      <c r="H73" s="12">
+        <v>2</v>
+      </c>
+      <c r="I73" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:9" ht="15.75">
-      <c r="A74" s="26"/>
-      <c r="B74" s="28"/>
+      <c r="A74" s="30"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
+      <c r="G74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H74" s="12">
+        <v>2</v>
+      </c>
+      <c r="I74" s="12">
+        <v>3</v>
+      </c>
     </row>
     <row r="75" spans="1:9" ht="15.75">
-      <c r="A75" s="26"/>
-      <c r="B75" s="28"/>
+      <c r="A75" s="30"/>
+      <c r="B75" s="27"/>
       <c r="C75" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
-      <c r="G75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="12">
+        <v>2</v>
+      </c>
+      <c r="I75" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="76" spans="1:9" ht="15.75">
-      <c r="A76" s="26"/>
-      <c r="B76" s="28"/>
-      <c r="C76" s="5" t="s">
-        <v>115</v>
+      <c r="A76" s="30"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
+      <c r="G76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="12">
+        <v>5</v>
+      </c>
+      <c r="I76" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="77" spans="1:9" ht="15.75">
-      <c r="A77" s="26"/>
-      <c r="B77" s="28"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="27"/>
       <c r="C77" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D77" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E77" s="2"/>
-      <c r="F77" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
+      <c r="H77" s="12">
+        <v>3</v>
+      </c>
+      <c r="I77" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:9" ht="15.75">
-      <c r="A78" s="26"/>
-      <c r="B78" s="28"/>
-      <c r="C78" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A78" s="30"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -2415,55 +2473,67 @@
       <c r="I78" s="12"/>
     </row>
     <row r="79" spans="1:9" ht="15.75">
-      <c r="A79" s="26"/>
-      <c r="B79" s="28"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="27"/>
       <c r="C79" s="10" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D79" s="2"/>
-      <c r="E79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="G79" s="2"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
+      <c r="H79" s="12">
+        <v>1</v>
+      </c>
+      <c r="I79" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:9" ht="15.75">
-      <c r="A80" s="26"/>
-      <c r="B80" s="28"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D80" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E80" s="2"/>
-      <c r="F80" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
+      <c r="H80" s="12">
+        <v>1</v>
+      </c>
+      <c r="I80" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="1:9" ht="15.75">
-      <c r="A81" s="26"/>
-      <c r="B81" s="28"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="27"/>
       <c r="C81" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="2"/>
+        <v>111</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
+      <c r="H81" s="12">
+        <v>1</v>
+      </c>
+      <c r="I81" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="1:9" ht="15.75">
-      <c r="A82" s="26"/>
-      <c r="B82" s="28"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -2471,145 +2541,183 @@
         <v>8</v>
       </c>
       <c r="G82" s="2"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
+      <c r="H82" s="12">
+        <v>1</v>
+      </c>
+      <c r="I82" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="83" spans="1:9" ht="15.75">
-      <c r="A83" s="26"/>
-      <c r="B83" s="28"/>
+      <c r="A83" s="30"/>
+      <c r="B83" s="27"/>
       <c r="C83" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D83" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E83" s="2"/>
-      <c r="F83" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
+      <c r="H83" s="12">
+        <v>1</v>
+      </c>
+      <c r="I83" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="1:9" ht="15.75">
-      <c r="A84" s="26"/>
-      <c r="B84" s="28"/>
+      <c r="A84" s="30"/>
+      <c r="B84" s="27"/>
       <c r="C84" s="10" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D84" s="2"/>
-      <c r="E84" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="G84" s="2"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
+      <c r="H84" s="12">
+        <v>2</v>
+      </c>
+      <c r="I84" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="85" spans="1:9" ht="15.75">
-      <c r="A85" s="26"/>
-      <c r="B85" s="28"/>
+      <c r="A85" s="30"/>
+      <c r="B85" s="27"/>
       <c r="C85" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85" s="2"/>
+      <c r="H85" s="12">
+        <v>2</v>
+      </c>
+      <c r="I85" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="15.75">
+      <c r="A86" s="30"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-    </row>
-    <row r="86" spans="1:9" ht="15.75">
-      <c r="A86" s="26"/>
-      <c r="B86" s="28"/>
-      <c r="C86" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
+      <c r="E86" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="12"/>
-      <c r="I86" s="12"/>
+      <c r="H86" s="12">
+        <v>1</v>
+      </c>
+      <c r="I86" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="87" spans="1:9" ht="15.75">
-      <c r="A87" s="26"/>
-      <c r="B87" s="28"/>
+      <c r="A87" s="30"/>
+      <c r="B87" s="27"/>
       <c r="C87" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E87" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
+      <c r="H87" s="12">
+        <v>1</v>
+      </c>
+      <c r="I87" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="88" spans="1:9" ht="15.75">
-      <c r="A88" s="26"/>
-      <c r="B88" s="28"/>
-      <c r="C88" s="10" t="s">
-        <v>124</v>
+      <c r="A88" s="30"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="D88" s="2"/>
-      <c r="E88" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
     </row>
     <row r="89" spans="1:9" ht="15.75">
-      <c r="A89" s="26"/>
-      <c r="B89" s="28"/>
+      <c r="A89" s="30"/>
+      <c r="B89" s="27"/>
       <c r="C89" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="12"/>
-      <c r="I89" s="12"/>
+      <c r="H89" s="12">
+        <v>2</v>
+      </c>
+      <c r="I89" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="90" spans="1:9" ht="15.75">
-      <c r="A90" s="26"/>
-      <c r="B90" s="28"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="27"/>
       <c r="C90" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E90" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="12"/>
+      <c r="H90" s="12">
+        <v>3</v>
+      </c>
+      <c r="I90" s="12">
+        <v>5</v>
+      </c>
     </row>
     <row r="91" spans="1:9" ht="15.75">
-      <c r="A91" s="26"/>
-      <c r="B91" s="28"/>
-      <c r="C91" s="5" t="s">
-        <v>126</v>
+      <c r="A91" s="30"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="12"/>
-      <c r="I91" s="12"/>
+      <c r="H91" s="12">
+        <v>2</v>
+      </c>
+      <c r="I91" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="92" spans="1:9" ht="15.75">
-      <c r="A92" s="26"/>
-      <c r="B92" s="28"/>
+      <c r="A92" s="30"/>
+      <c r="B92" s="27"/>
       <c r="C92" s="10" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>8</v>
@@ -2617,18 +2725,20 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="12"/>
-      <c r="I92" s="12"/>
+      <c r="H92" s="12">
+        <v>2</v>
+      </c>
+      <c r="I92" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="93" spans="1:9" ht="15.75">
-      <c r="A93" s="26"/>
-      <c r="B93" s="28"/>
-      <c r="C93" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A93" s="30"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -2636,10 +2746,10 @@
       <c r="I93" s="12"/>
     </row>
     <row r="94" spans="1:9" ht="15.75">
-      <c r="A94" s="26"/>
-      <c r="B94" s="28"/>
+      <c r="A94" s="30"/>
+      <c r="B94" s="27"/>
       <c r="C94" s="10" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>8</v>
@@ -2647,29 +2757,37 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="12"/>
-      <c r="I94" s="12"/>
-    </row>
-    <row r="95" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A95" s="26"/>
-      <c r="B95" s="28"/>
-      <c r="C95" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D95" s="2"/>
+      <c r="H94" s="12">
+        <v>2</v>
+      </c>
+      <c r="I94" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="15.75">
+      <c r="A95" s="30"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E95" s="2"/>
-      <c r="F95" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="12"/>
-      <c r="I95" s="12"/>
+      <c r="H95" s="12">
+        <v>1</v>
+      </c>
+      <c r="I95" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="96" spans="1:9" ht="15.75">
-      <c r="A96" s="26"/>
-      <c r="B96" s="28"/>
-      <c r="C96" s="4" t="s">
-        <v>73</v>
+      <c r="A96" s="30"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>8</v>
@@ -2677,27 +2795,33 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="12"/>
-      <c r="I96" s="12"/>
-    </row>
-    <row r="97" spans="1:9" ht="15.75">
-      <c r="A97" s="26"/>
-      <c r="B97" s="28"/>
-      <c r="C97" s="22" t="s">
-        <v>74</v>
+      <c r="H96" s="12">
+        <v>2</v>
+      </c>
+      <c r="I96" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A97" s="30"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
+      <c r="F97" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="G97" s="2"/>
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
     </row>
     <row r="98" spans="1:9" ht="15.75">
-      <c r="A98" s="26"/>
-      <c r="B98" s="28"/>
-      <c r="C98" s="10" t="s">
-        <v>75</v>
+      <c r="A98" s="30"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>8</v>
@@ -2709,14 +2833,12 @@
       <c r="I98" s="12"/>
     </row>
     <row r="99" spans="1:9" ht="15.75">
-      <c r="A99" s="26"/>
-      <c r="B99" s="28"/>
-      <c r="C99" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A99" s="30"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -2724,12 +2846,14 @@
       <c r="I99" s="12"/>
     </row>
     <row r="100" spans="1:9" ht="15.75">
-      <c r="A100" s="26"/>
-      <c r="B100" s="28"/>
-      <c r="C100" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D100" s="2"/>
+      <c r="A100" s="30"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -2737,10 +2861,10 @@
       <c r="I100" s="12"/>
     </row>
     <row r="101" spans="1:9" ht="15.75">
-      <c r="A101" s="26"/>
-      <c r="B101" s="28"/>
+      <c r="A101" s="30"/>
+      <c r="B101" s="27"/>
       <c r="C101" s="10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>8</v>
@@ -2752,14 +2876,12 @@
       <c r="I101" s="12"/>
     </row>
     <row r="102" spans="1:9" ht="15.75">
-      <c r="A102" s="26"/>
-      <c r="B102" s="28"/>
-      <c r="C102" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A102" s="30"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -2767,12 +2889,14 @@
       <c r="I102" s="12"/>
     </row>
     <row r="103" spans="1:9" ht="15.75">
-      <c r="A103" s="26"/>
-      <c r="B103" s="28"/>
-      <c r="C103" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D103" s="2"/>
+      <c r="A103" s="30"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -2780,29 +2904,27 @@
       <c r="I103" s="12"/>
     </row>
     <row r="104" spans="1:9" ht="15.75">
-      <c r="A104" s="26"/>
-      <c r="B104" s="28"/>
+      <c r="A104" s="30"/>
+      <c r="B104" s="27"/>
       <c r="C104" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D104" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E104" s="2"/>
-      <c r="F104" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
     </row>
     <row r="105" spans="1:9" ht="15.75">
-      <c r="A105" s="26"/>
-      <c r="B105" s="28"/>
-      <c r="C105" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A105" s="30"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
@@ -2810,15 +2932,13 @@
       <c r="I105" s="12"/>
     </row>
     <row r="106" spans="1:9" ht="15.75">
-      <c r="A106" s="26"/>
-      <c r="B106" s="28"/>
+      <c r="A106" s="30"/>
+      <c r="B106" s="27"/>
       <c r="C106" s="10" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D106" s="2"/>
-      <c r="E106" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E106" s="2"/>
       <c r="F106" s="2" t="s">
         <v>8</v>
       </c>
@@ -2827,97 +2947,95 @@
       <c r="I106" s="12"/>
     </row>
     <row r="107" spans="1:9" ht="15.75">
-      <c r="A107" s="26"/>
-      <c r="B107" s="28"/>
+      <c r="A107" s="30"/>
+      <c r="B107" s="27"/>
       <c r="C107" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
     </row>
     <row r="108" spans="1:9" ht="15.75">
-      <c r="A108" s="31"/>
-      <c r="B108" s="29"/>
+      <c r="A108" s="30"/>
+      <c r="B108" s="27"/>
       <c r="C108" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D108" s="2"/>
       <c r="E108" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="G108" s="2"/>
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
     </row>
-    <row r="109" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A109" s="30">
-        <v>6</v>
-      </c>
-      <c r="B109" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C109" s="22" t="s">
-        <v>19</v>
+    <row r="109" spans="1:9" ht="15.75">
+      <c r="A109" s="30"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
+      <c r="E109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
     </row>
     <row r="110" spans="1:9" ht="15.75">
-      <c r="A110" s="26"/>
+      <c r="A110" s="31"/>
       <c r="B110" s="28"/>
       <c r="C110" s="10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E110" s="2"/>
+      <c r="E110" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F110" s="2"/>
-      <c r="G110" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="G110" s="2"/>
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
     </row>
-    <row r="111" spans="1:9" ht="15.75">
-      <c r="A111" s="26"/>
-      <c r="B111" s="28"/>
-      <c r="C111" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>8</v>
-      </c>
+    <row r="111" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A111" s="29">
+        <v>6</v>
+      </c>
+      <c r="B111" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
-      <c r="G111" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="G111" s="2"/>
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
     </row>
     <row r="112" spans="1:9" ht="15.75">
-      <c r="A112" s="26"/>
-      <c r="B112" s="28"/>
+      <c r="A112" s="30"/>
+      <c r="B112" s="27"/>
       <c r="C112" s="10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>8</v>
@@ -2931,31 +3049,33 @@
       <c r="I112" s="12"/>
     </row>
     <row r="113" spans="1:9" ht="15.75">
-      <c r="A113" s="26"/>
-      <c r="B113" s="28"/>
-      <c r="C113" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D113" s="2"/>
+      <c r="A113" s="30"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
+      <c r="G113" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
     </row>
     <row r="114" spans="1:9" ht="15.75">
-      <c r="A114" s="26"/>
-      <c r="B114" s="28"/>
+      <c r="A114" s="30"/>
+      <c r="B114" s="27"/>
       <c r="C114" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
       <c r="G114" s="2" t="s">
         <v>8</v>
       </c>
@@ -2963,113 +3083,113 @@
       <c r="I114" s="12"/>
     </row>
     <row r="115" spans="1:9" ht="15.75">
-      <c r="A115" s="26"/>
-      <c r="B115" s="28"/>
-      <c r="C115" s="10" t="s">
-        <v>90</v>
+      <c r="A115" s="30"/>
+      <c r="B115" s="27"/>
+      <c r="C115" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="D115" s="2"/>
-      <c r="E115" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
     </row>
     <row r="116" spans="1:9" ht="15.75">
-      <c r="A116" s="26"/>
-      <c r="B116" s="28"/>
+      <c r="A116" s="30"/>
+      <c r="B116" s="27"/>
       <c r="C116" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H116" s="12"/>
       <c r="I116" s="12"/>
     </row>
     <row r="117" spans="1:9" ht="15.75">
-      <c r="A117" s="31"/>
-      <c r="B117" s="29"/>
-      <c r="C117" s="23" t="s">
-        <v>92</v>
+      <c r="A117" s="30"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
+      <c r="E117" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F117" s="2"/>
-      <c r="G117" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="G117" s="2"/>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
     </row>
-    <row r="118" spans="1:9">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="I118" s="3"/>
-    </row>
-    <row r="119" spans="1:9">
-      <c r="A119" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B119" s="3"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="I119" s="3"/>
+    <row r="118" spans="1:9" ht="15.75">
+      <c r="A118" s="30"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="12"/>
+      <c r="I118" s="12"/>
+    </row>
+    <row r="119" spans="1:9" ht="15.75">
+      <c r="A119" s="31"/>
+      <c r="B119" s="28"/>
+      <c r="C119" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H119" s="12"/>
+      <c r="I119" s="12"/>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="I120" s="3"/>
     </row>
-    <row r="121" spans="1:9" ht="60">
-      <c r="A121" s="18">
-        <v>1</v>
-      </c>
-      <c r="B121" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C121" s="4">
-        <v>1</v>
-      </c>
+    <row r="121" spans="1:9">
+      <c r="A121" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B121" s="3"/>
+      <c r="C121" s="1"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
       <c r="I121" s="3"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
-      <c r="A122" s="20">
-        <v>2</v>
-      </c>
-      <c r="B122" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C122" s="20">
-        <v>2</v>
+    <row r="122" spans="1:9">
+      <c r="A122" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
@@ -3077,15 +3197,15 @@
       <c r="G122" s="3"/>
       <c r="I122" s="3"/>
     </row>
-    <row r="123" spans="1:9" ht="30">
-      <c r="A123" s="20">
-        <v>3</v>
+    <row r="123" spans="1:9" ht="60">
+      <c r="A123" s="18">
+        <v>1</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C123" s="20">
-        <v>3</v>
+        <v>29</v>
+      </c>
+      <c r="C123" s="4">
+        <v>1</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
@@ -3095,13 +3215,13 @@
     </row>
     <row r="124" spans="1:9" ht="30">
       <c r="A124" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C124" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
@@ -3111,13 +3231,13 @@
     </row>
     <row r="125" spans="1:9" ht="30">
       <c r="A125" s="20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C125" s="20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
@@ -3125,14 +3245,32 @@
       <c r="G125" s="3"/>
       <c r="I125" s="3"/>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" ht="30">
+      <c r="A126" s="20">
+        <v>4</v>
+      </c>
+      <c r="B126" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C126" s="20">
+        <v>4</v>
+      </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="I126" s="3"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" ht="30">
+      <c r="A127" s="20">
+        <v>5</v>
+      </c>
+      <c r="B127" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" s="20">
+        <v>5</v>
+      </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
@@ -3209,23 +3347,37 @@
       <c r="G137" s="3"/>
       <c r="I137" s="3"/>
     </row>
+    <row r="138" spans="4:9">
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+      <c r="I138" s="3"/>
+    </row>
+    <row r="139" spans="4:9">
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+      <c r="I139" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B33:B61"/>
+    <mergeCell ref="A33:A61"/>
+    <mergeCell ref="A111:A119"/>
+    <mergeCell ref="B111:B119"/>
+    <mergeCell ref="A62:A110"/>
+    <mergeCell ref="B62:B110"/>
     <mergeCell ref="B11:B20"/>
     <mergeCell ref="B21:B32"/>
     <mergeCell ref="A21:A32"/>
     <mergeCell ref="A11:A20"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B33:B61"/>
-    <mergeCell ref="A33:A61"/>
-    <mergeCell ref="A109:A117"/>
-    <mergeCell ref="B109:B117"/>
-    <mergeCell ref="A62:A108"/>
-    <mergeCell ref="B62:B108"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D36 F2:F36 F38:F61 G2:G61 E2:E61 D38:D61 D62:G135">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D36 F2:F36 F38:F61 G2:G61 E2:E61 D38:D61 D62:G137">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>